<commit_message>
Add Auswertung + Anfang doku Numerical Methods
</commit_message>
<xml_diff>
--- a/Auswertungen/EnergieVerlustVergleich.xlsx
+++ b/Auswertungen/EnergieVerlustVergleich.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\3 Schule\Next\Auswertungen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-Repos\simulation\Auswertungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A14737-AE40-41AA-A380-F5FB4DDF0CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DB3ED3B1-9FAF-4FC8-B164-7AFB9A45769F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Vergleich" sheetId="1" r:id="rId1"/>
     <sheet name="NASA Vergleich" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="33">
   <si>
     <t>Euler:</t>
   </si>
@@ -34,9 +33,6 @@
     <t>runge Kutta:</t>
   </si>
   <si>
-    <t>leapfrog:</t>
-  </si>
-  <si>
     <t>deltaTime</t>
   </si>
   <si>
@@ -98,12 +94,42 @@
   </si>
   <si>
     <t>ss</t>
+  </si>
+  <si>
+    <t>Calculations</t>
+  </si>
+  <si>
+    <t>-0,001%</t>
+  </si>
+  <si>
+    <t>-2,26E-5%</t>
+  </si>
+  <si>
+    <t>DKD leapfrog:</t>
+  </si>
+  <si>
+    <t>KDK Leapfrog</t>
+  </si>
+  <si>
+    <t>partikel nach Partikel</t>
+  </si>
+  <si>
+    <t>-2,35E-10%</t>
+  </si>
+  <si>
+    <t>-0,000000000024%</t>
+  </si>
+  <si>
+    <t>-0,0000000019%</t>
+  </si>
+  <si>
+    <t>-1,766E-11%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000%"/>
@@ -404,7 +430,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -449,6 +475,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Ausgabe" xfId="6" builtinId="21"/>
@@ -768,26 +798,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B721DBF9-AE77-4BFB-BF9C-ABE22F67535F}">
-  <dimension ref="A2:R31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AB31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
     <col min="11" max="11" width="23.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" customWidth="1"/>
+    <col min="22" max="22" width="14" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
@@ -795,22 +829,25 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="14" t="s">
+      <c r="I4" s="13"/>
+      <c r="J4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
-      <c r="N4" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -828,48 +865,65 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
       <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" t="s">
-        <v>4</v>
+      <c r="H9" t="s">
+        <v>23</v>
       </c>
       <c r="J9" t="s">
         <v>3</v>
       </c>
       <c r="K9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
         <v>4</v>
+      </c>
+      <c r="N9" t="s">
+        <v>23</v>
       </c>
       <c r="P9" t="s">
         <v>3</v>
       </c>
       <c r="Q9" t="s">
-        <v>5</v>
-      </c>
-      <c r="R9" s="5"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="R9" t="s">
+        <v>4</v>
+      </c>
+      <c r="T9" t="s">
+        <v>3</v>
+      </c>
+      <c r="U9" t="s">
+        <v>2</v>
+      </c>
+      <c r="V9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
       <c r="D10">
         <v>10</v>
@@ -880,24 +934,41 @@
       <c r="F10" s="6">
         <v>-8.6368983495103798E+30</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>10</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>100000</v>
       </c>
-      <c r="O10">
+      <c r="L10">
+        <f>-2.29E+31</f>
+        <v>-2.29E+31</v>
+      </c>
+      <c r="M10" s="40">
+        <v>-8.5000000000000006E-3</v>
+      </c>
+      <c r="N10" s="42"/>
+      <c r="P10">
         <v>10</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>100000</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="R10" s="6">
         <v>3.3018388667247001E+27</v>
       </c>
-      <c r="R10" s="5"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <v>10</v>
+      </c>
+      <c r="U10">
+        <v>100000</v>
+      </c>
+      <c r="W10" s="41"/>
+      <c r="X10" s="42"/>
+      <c r="AA10" s="40"/>
+      <c r="AB10" s="42"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
       <c r="D11">
         <v>100</v>
@@ -908,24 +979,50 @@
       <c r="F11" s="6">
         <v>-1.05465784151321E+30</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>100</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>10000</v>
       </c>
-      <c r="O11">
+      <c r="L11" s="8">
+        <v>-2.7900000000000001E+30</v>
+      </c>
+      <c r="M11" s="40">
+        <v>-1E-3</v>
+      </c>
+      <c r="N11" s="42">
+        <v>792</v>
+      </c>
+      <c r="P11">
         <v>100</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>10000</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="R11" s="7">
         <v>-2.5090178695766899E+26</v>
       </c>
-      <c r="R11" s="5"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>100</v>
+      </c>
+      <c r="U11">
+        <v>10000</v>
+      </c>
+      <c r="V11" s="8">
+        <v>5.2200000000000002E+24</v>
+      </c>
+      <c r="W11" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="X11" s="42">
+        <v>396</v>
+      </c>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="42"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
       <c r="D12">
         <v>1000</v>
@@ -936,25 +1033,44 @@
       <c r="F12" s="6">
         <v>-1.0764205093716899E+29</v>
       </c>
-      <c r="I12">
-        <v>1000</v>
-      </c>
       <c r="J12">
         <v>1000</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="O12">
+      <c r="K12">
         <v>1000</v>
+      </c>
+      <c r="L12" s="8">
+        <v>-2.84E+29</v>
+      </c>
+      <c r="M12" s="40">
+        <v>-1E-4</v>
+      </c>
+      <c r="N12" s="42">
+        <v>7992</v>
       </c>
       <c r="P12">
         <v>1000</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12">
+        <v>1000</v>
+      </c>
+      <c r="R12" s="9">
         <v>-3.1410744913864503E+26</v>
       </c>
-      <c r="R12" s="5"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T12">
+        <v>1000</v>
+      </c>
+      <c r="U12">
+        <v>1000</v>
+      </c>
+      <c r="V12" s="8"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="42"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="40"/>
+      <c r="AB12" s="42"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
       <c r="D13">
         <v>10000</v>
@@ -965,24 +1081,50 @@
       <c r="F13" s="9">
         <v>-1.1067427619372699E+28</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>10000</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>100</v>
       </c>
-      <c r="O13">
+      <c r="L13" s="8">
+        <v>-2.8799999999999999E+28</v>
+      </c>
+      <c r="M13" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="42">
+        <v>79992</v>
+      </c>
+      <c r="P13">
         <v>10000</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>100</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="R13" s="9">
         <v>-3.1577904120513702E+26</v>
       </c>
-      <c r="R13" s="5"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <v>10000</v>
+      </c>
+      <c r="U13">
+        <v>100</v>
+      </c>
+      <c r="V13" s="8">
+        <v>6.4199999999999998E+22</v>
+      </c>
+      <c r="W13" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="X13" s="42">
+        <v>39996</v>
+      </c>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="41"/>
+      <c r="AB13" s="42"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C14" s="4"/>
       <c r="D14">
         <v>100000</v>
@@ -993,24 +1135,56 @@
       <c r="F14" s="9">
         <v>-1.39125116563088E+27</v>
       </c>
-      <c r="I14">
+      <c r="G14" s="8">
+        <v>-5.1999999999999997E-5</v>
+      </c>
+      <c r="H14">
+        <v>199998</v>
+      </c>
+      <c r="J14">
         <v>100000</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>10</v>
       </c>
-      <c r="O14">
+      <c r="L14" s="8">
+        <v>-3.17E+27</v>
+      </c>
+      <c r="M14" s="41">
+        <v>-9.9999999999999995E-7</v>
+      </c>
+      <c r="N14" s="42">
+        <v>799992</v>
+      </c>
+      <c r="P14">
         <v>100000</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>10</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="R14" s="9">
         <v>-3.1589778693196503E+26</v>
       </c>
-      <c r="R14" s="5"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T14">
+        <v>100000</v>
+      </c>
+      <c r="U14">
+        <v>10</v>
+      </c>
+      <c r="V14" s="8">
+        <v>6.2700000000000005E+21</v>
+      </c>
+      <c r="W14" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="X14" s="42">
+        <v>399996</v>
+      </c>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="41"/>
+      <c r="AB14" s="42"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
       <c r="D15">
         <v>1000000</v>
@@ -1021,24 +1195,47 @@
       <c r="F15" s="7">
         <v>-4.2344627093166798E+26</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>1000000</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>1</v>
       </c>
-      <c r="O15">
+      <c r="L15" s="8">
+        <v>-6.0569999999999999E+26</v>
+      </c>
+      <c r="M15" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="42">
+        <v>7999992</v>
+      </c>
+      <c r="P15">
         <v>1000000</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>1</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="R15" s="9">
         <v>-3.1589778693196503E+26</v>
       </c>
-      <c r="R15" s="5"/>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T15">
+        <v>1000000</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15" s="8">
+        <v>4.715E+20</v>
+      </c>
+      <c r="W15" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="X15" s="42">
+        <v>3999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
@@ -1049,7 +1246,7 @@
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="M16" s="43"/>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
@@ -1077,7 +1274,7 @@
     </row>
     <row r="19" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R19" s="5"/>
     </row>
@@ -1088,31 +1285,31 @@
     <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
       <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
         <v>4</v>
       </c>
-      <c r="E21" t="s">
+      <c r="I21" t="s">
         <v>3</v>
       </c>
-      <c r="F21" t="s">
-        <v>5</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" t="s">
         <v>4</v>
       </c>
-      <c r="J21" t="s">
+      <c r="O21" t="s">
         <v>3</v>
       </c>
-      <c r="K21" t="s">
-        <v>5</v>
-      </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" t="s">
         <v>4</v>
-      </c>
-      <c r="P21" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>5</v>
       </c>
       <c r="R21" s="5"/>
     </row>
@@ -1275,11 +1472,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9757DFD2-04D7-4074-A8E6-86A76DA00322}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1492,7 @@
     <row r="1" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="28">
         <v>43831</v>
@@ -1311,7 +1508,7 @@
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="8">
         <v>-25453343414.131401</v>
@@ -1327,7 +1524,7 @@
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8">
         <v>146091299360.686</v>
@@ -1343,7 +1540,7 @@
     </row>
     <row r="5" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="22">
         <v>-2712536.2576693301</v>
@@ -1364,7 +1561,7 @@
     </row>
     <row r="7" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1377,7 +1574,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="35"/>
       <c r="N7" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -1393,19 +1590,19 @@
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="24">
         <v>86400</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="16">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="2"/>
@@ -1414,19 +1611,19 @@
       <c r="L8" s="36"/>
       <c r="N8" s="36"/>
       <c r="O8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P8" s="24">
         <v>86400</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R8" s="16">
         <v>1</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T8" s="16"/>
       <c r="U8" s="2"/>
@@ -1470,7 +1667,7 @@
       </c>
       <c r="I11" s="31"/>
       <c r="J11" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L11" s="36"/>
       <c r="N11" s="36"/>
@@ -1487,7 +1684,7 @@
       </c>
       <c r="U11" s="31"/>
       <c r="V11" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
@@ -1495,7 +1692,7 @@
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="8">
         <v>-25453343414.131401</v>
@@ -1518,7 +1715,7 @@
       <c r="L12" s="37"/>
       <c r="N12" s="36"/>
       <c r="O12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P12" s="8">
         <v>-25453343414.131401</v>
@@ -1543,7 +1740,7 @@
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="8">
         <v>146091299360.686</v>
@@ -1560,7 +1757,7 @@
       <c r="L13" s="36"/>
       <c r="N13" s="36"/>
       <c r="O13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P13" s="8">
         <v>146091299360.686</v>
@@ -1580,7 +1777,7 @@
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="8">
         <v>-2712536.2576693301</v>
@@ -1594,7 +1791,7 @@
       <c r="L14" s="36"/>
       <c r="N14" s="36"/>
       <c r="O14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P14" s="8">
         <v>-2712536.2576693301</v>
@@ -1619,40 +1816,40 @@
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16">
         <f>SQRT(($F$3-F12)^2+($F$4-F13)^2+($F$5-F14)^2)</f>
         <v>2096914241.9227929</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16">
         <f>SQRT(($H$3-H12)^2+($H$4-H13)^2+($H$5-H14)^2)</f>
         <v>4202497816.9329267</v>
       </c>
       <c r="I16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L16" s="36"/>
       <c r="N16" s="36"/>
       <c r="O16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R16">
         <f>SQRT(($F$3-R12)^2+($F$4-R13)^2+($F$5-R14)^2)</f>
         <v>1951165876.3430951</v>
       </c>
       <c r="S16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T16">
         <f>SQRT(($H$3-T12)^2+($H$4-T13)^2+($H$5-T14)^2)</f>
         <v>3907441567.4765611</v>
       </c>
       <c r="U16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
@@ -1665,14 +1862,14 @@
         <v>2096914.241922793</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" s="18">
         <f>H16/1000</f>
         <v>4202497.8169329269</v>
       </c>
       <c r="I17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L17" s="36"/>
       <c r="N17" s="36"/>
@@ -1681,14 +1878,14 @@
         <v>1951165.876343095</v>
       </c>
       <c r="S17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T17" s="18">
         <f>T16/1000</f>
         <v>3907441.5674765613</v>
       </c>
       <c r="U17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
@@ -1744,19 +1941,19 @@
     <row r="21" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2">
         <v>3600</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21" s="16">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="2"/>
@@ -1765,19 +1962,19 @@
       <c r="L21" s="36"/>
       <c r="N21" s="36"/>
       <c r="O21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P21" s="2">
         <v>3600</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R21" s="16">
         <v>1</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T21" s="16"/>
       <c r="U21" s="2"/>
@@ -1821,7 +2018,7 @@
       </c>
       <c r="I24" s="31"/>
       <c r="J24" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L24" s="36"/>
       <c r="N24" s="36"/>
@@ -1838,7 +2035,7 @@
       </c>
       <c r="U24" s="31"/>
       <c r="V24" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
@@ -1846,7 +2043,7 @@
     <row r="25" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" s="8">
         <v>-25453343414.131401</v>
@@ -1869,7 +2066,7 @@
       <c r="L25" s="37"/>
       <c r="N25" s="36"/>
       <c r="O25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P25" s="8">
         <v>-25453343414.131401</v>
@@ -1894,7 +2091,7 @@
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26" s="8">
         <v>146091299360.686</v>
@@ -1911,7 +2108,7 @@
       <c r="L26" s="36"/>
       <c r="N26" s="36"/>
       <c r="O26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P26" s="8">
         <v>146091299360.686</v>
@@ -1931,7 +2128,7 @@
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="8">
         <v>-2712536.2576693301</v>
@@ -1945,7 +2142,7 @@
       <c r="L27" s="36"/>
       <c r="N27" s="36"/>
       <c r="O27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P27" s="8">
         <v>-2712536.2576693301</v>
@@ -1970,40 +2167,40 @@
     <row r="29" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F29">
         <f>SQRT(($F$3-F25)^2+($F$4-F26)^2+($F$5-F27)^2)</f>
         <v>1858859195.3445516</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H29">
         <f>SQRT(($H$3-H25)^2+($H$4-H26)^2+($H$5-H27)^2)</f>
         <v>3723238248.2321258</v>
       </c>
       <c r="I29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L29" s="36"/>
       <c r="N29" s="36"/>
       <c r="O29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R29">
         <f>SQRT(($F$3-R25)^2+($F$4-R26)^2+($F$5-R27)^2)</f>
         <v>1857386791.6498744</v>
       </c>
       <c r="S29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T29">
         <f>SQRT(($H$3-T25)^2+($H$4-T26)^2+($H$5-T27)^2)</f>
         <v>3720190377.4916215</v>
       </c>
       <c r="U29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
@@ -2016,14 +2213,14 @@
         <v>1858859.1953445515</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" s="18">
         <f>H29/1000</f>
         <v>3723238.2482321258</v>
       </c>
       <c r="I30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L30" s="36"/>
       <c r="N30" s="36"/>
@@ -2032,14 +2229,14 @@
         <v>1857386.7916498745</v>
       </c>
       <c r="S30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T30" s="18">
         <f>T29/1000</f>
         <v>3720190.3774916213</v>
       </c>
       <c r="U30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
@@ -2113,13 +2310,13 @@
     <row r="34" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
       <c r="C34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" s="2">
         <v>1000</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="2"/>
@@ -2130,19 +2327,19 @@
       <c r="L34" s="38"/>
       <c r="N34" s="38"/>
       <c r="O34" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P34" s="2">
         <v>1000</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R34" s="16">
         <v>1</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T34" s="16"/>
       <c r="U34" s="2"/>
@@ -2190,7 +2387,7 @@
       </c>
       <c r="I37" s="31"/>
       <c r="J37" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
@@ -2210,7 +2407,7 @@
       </c>
       <c r="U37" s="31"/>
       <c r="V37" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W37" s="5"/>
       <c r="X37" s="34"/>
@@ -2218,7 +2415,7 @@
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="C38" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D38" s="8">
         <v>-25453343414.131401</v>
@@ -2241,7 +2438,7 @@
       <c r="L38" s="25"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P38" s="8">
         <v>-25453343414.131401</v>
@@ -2266,7 +2463,7 @@
     <row r="39" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D39" s="8">
         <v>146091299360.686</v>
@@ -2284,7 +2481,7 @@
       <c r="L39" s="5"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P39" s="8">
         <v>146091299360.686</v>
@@ -2304,7 +2501,7 @@
     <row r="40" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D40" s="8">
         <v>-2712536.2576693301</v>
@@ -2319,7 +2516,7 @@
       <c r="L40" s="5"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P40" s="8">
         <v>-2712536.2576693301</v>
@@ -2346,41 +2543,41 @@
     <row r="42" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F42">
         <f>SQRT(($F$3-F38)^2+($F$4-F39)^2+($F$5-F40)^2)</f>
         <v>1839415232.0926788</v>
       </c>
       <c r="G42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H42">
         <f>SQRT(($H$3-H38)^2+($H$4-H39)^2+($H$5-H40)^2)</f>
         <v>3702475741.747838</v>
       </c>
       <c r="I42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R42">
         <f>SQRT(($F$3-R38)^2+($F$4-R39)^2+($F$5-R40)^2)</f>
         <v>1839149228.6461191</v>
       </c>
       <c r="S42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T42">
         <f>SQRT(($H$3-T38)^2+($H$4-T39)^2+($H$5-T40)^2)</f>
         <v>3701728246.7136521</v>
       </c>
       <c r="U42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W42" s="5"/>
       <c r="X42" s="5"/>
@@ -2393,14 +2590,14 @@
         <v>1839415.2320926788</v>
       </c>
       <c r="G43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H43" s="18">
         <f>H42/1000</f>
         <v>3702475.741747838</v>
       </c>
       <c r="I43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
@@ -2411,14 +2608,14 @@
         <v>1839149.2286461191</v>
       </c>
       <c r="S43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T43" s="18">
         <f>T42/1000</f>
         <v>3701728.2467136523</v>
       </c>
       <c r="U43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W43" s="5"/>
       <c r="X43" s="5"/>
@@ -2492,13 +2689,13 @@
     <row r="47" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4"/>
       <c r="C47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" s="2">
         <v>500</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F47" s="16"/>
       <c r="G47" s="2"/>
@@ -2509,13 +2706,13 @@
       <c r="L47" s="38"/>
       <c r="N47" s="4"/>
       <c r="O47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P47" s="2">
         <v>500</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R47" s="16"/>
       <c r="S47" s="2"/>
@@ -2565,7 +2762,7 @@
       </c>
       <c r="I50" s="31"/>
       <c r="J50" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
@@ -2584,7 +2781,7 @@
       </c>
       <c r="U50" s="31"/>
       <c r="V50" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W50" s="5"/>
       <c r="X50" s="5"/>
@@ -2592,7 +2789,7 @@
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D51" s="8">
         <v>-25453343414.131401</v>
@@ -2615,7 +2812,7 @@
       <c r="L51" s="25"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P51" s="8">
         <v>-25453343414.131401</v>
@@ -2640,7 +2837,7 @@
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D52" s="8">
         <v>146091299360.686</v>
@@ -2658,7 +2855,7 @@
       <c r="L52" s="5"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P52" s="8">
         <v>146091299360.686</v>
@@ -2678,7 +2875,7 @@
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D53" s="8">
         <v>-2712536.2576693301</v>
@@ -2693,7 +2890,7 @@
       <c r="L53" s="5"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P53" s="8">
         <v>-2712536.2576693301</v>
@@ -2720,41 +2917,41 @@
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
       <c r="C55" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F55">
         <f>SQRT(($F$3-F51)^2+($F$4-F52)^2+($F$5-F53)^2)</f>
         <v>1854367075.111536</v>
       </c>
       <c r="G55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H55">
         <f>SQRT(($H$3-H51)^2+($H$4-H52)^2+($H$5-H53)^2)</f>
         <v>3717208905.3091784</v>
       </c>
       <c r="I55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="N55" s="4"/>
       <c r="O55" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R55">
         <f>SQRT(($F$3-R51)^2+($F$4-R52)^2+($F$5-R53)^2)</f>
         <v>672853950.2313627</v>
       </c>
       <c r="S55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T55">
         <f>SQRT(($H$3-T51)^2+($H$4-T52)^2+($H$5-T53)^2)</f>
         <v>1309162471.1822069</v>
       </c>
       <c r="U55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W55" s="5"/>
       <c r="X55" s="5"/>
@@ -2767,14 +2964,14 @@
         <v>1854367.0751115361</v>
       </c>
       <c r="G56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H56" s="18">
         <f>H55/1000</f>
         <v>3717208.9053091784</v>
       </c>
       <c r="I56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
@@ -2785,14 +2982,14 @@
         <v>672853.95023136272</v>
       </c>
       <c r="S56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T56" s="18">
         <f>T55/1000</f>
         <v>1309162.4711822069</v>
       </c>
       <c r="U56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W56" s="5"/>
       <c r="X56" s="5"/>
@@ -2859,7 +3056,7 @@
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2943,7 +3140,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H57 F57 R57 T57 R44 T44 F44 H44 F18 H18 R18">
+  <conditionalFormatting sqref="F57 H57 R57 T57 R44 T44 F44 H44 F18 H18 R18">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>